<commit_message>
added keyboard letters and blank spaces
</commit_message>
<xml_diff>
--- a/players_info.xlsx
+++ b/players_info.xlsx
@@ -5065,13 +5065,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5122,13 +5128,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="17" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -5141,13 +5147,13 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="17" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5468,7 +5474,7 @@
     <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5497,7 +5503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -5526,7 +5532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="44.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="46.5">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -5555,7 +5561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="44.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="46.5">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -5584,7 +5590,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="44.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="46.5">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -5613,7 +5619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="44.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="46.5">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -5642,7 +5648,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="57">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="60">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -5671,7 +5677,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="44.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="46.5">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -5700,7 +5706,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="44.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="46.5">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>

</xml_diff>